<commit_message>
Inserted the timing data into excel
</commit_message>
<xml_diff>
--- a/graphs/Timinganalysis.xlsx
+++ b/graphs/Timinganalysis.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GCC" sheetId="3" r:id="rId1"/>
     <sheet name="Emacs" sheetId="4" r:id="rId2"/>
     <sheet name="20MB File" sheetId="5" r:id="rId3"/>
+    <sheet name="100MB file" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
@@ -7384,7 +7385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
@@ -10861,4 +10862,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>